<commit_message>
sheet 2 and 3
</commit_message>
<xml_diff>
--- a/Inventory list.xlsx
+++ b/Inventory list.xlsx
@@ -7,12 +7,14 @@
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
-    <sheet name="Inventory List" sheetId="1" r:id="rId1"/>
+    <sheet name="Supplies" sheetId="1" r:id="rId1"/>
+    <sheet name="CCL" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inventory List'!$J$2</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Inventory List'!$1:$3</definedName>
-    <definedName name="valHighlight">IFERROR(IF('Inventory List'!$K$2="Yes", TRUE, FALSE),FALSE)</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Supplies!$K$2</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Supplies!$1:$3</definedName>
+    <definedName name="valHighlight">IFERROR(IF(Supplies!$L$2="Yes", TRUE, FALSE),FALSE)</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
   <si>
     <t>Highlight items to reorder?</t>
   </si>
@@ -67,9 +69,6 @@
     <t>Discontinued?</t>
   </si>
   <si>
-    <t>Item 2</t>
-  </si>
-  <si>
     <t>Item 3</t>
   </si>
   <si>
@@ -116,6 +115,63 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wireless Mouse </t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Purchase Date</t>
+  </si>
+  <si>
+    <t>Warranty Expiry Date</t>
+  </si>
+  <si>
+    <t>Date Set Up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location </t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>PC NO.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mouse </t>
+  </si>
+  <si>
+    <t>Monitor</t>
+  </si>
+  <si>
+    <t>System Unit</t>
+  </si>
+  <si>
+    <t>AVR</t>
+  </si>
+  <si>
+    <t>Care of</t>
+  </si>
+  <si>
+    <t>DCS</t>
+  </si>
+  <si>
+    <t>Sir Nico</t>
   </si>
 </sst>
 </file>
@@ -183,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -250,6 +306,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -260,7 +319,38 @@
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="33">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD1FFBD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color theme="1" tint="0.34998626667073579"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -294,6 +384,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -308,7 +416,11 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -318,11 +430,16 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="[$₱-3409]#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -332,11 +449,16 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="[$₱-3409]#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -346,7 +468,62 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="[$₱-3409]#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -375,6 +552,97 @@
         <name val="Franklin Gothic Book"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF339933"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -391,6 +659,53 @@
       </font>
       <numFmt numFmtId="164" formatCode="[$₱-3409]#,##0.00"/>
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$₱-3409]#,##0.00"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Franklin Gothic Book"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -520,9 +835,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Business Table" pivot="0" count="3">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="32"/>
+      <tableStyleElement type="headerRow" dxfId="31"/>
+      <tableStyleElement type="secondRowStripe" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -548,16 +863,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>514350</xdr:rowOff>
+      <xdr:rowOff>1386840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>981074</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1737360</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -572,8 +887,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="152399" y="514350"/>
-          <a:ext cx="1986915" cy="956310"/>
+          <a:off x="4030979" y="1386840"/>
+          <a:ext cx="2354581" cy="350520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -603,38 +918,26 @@
         <a:p>
           <a:pPr marL="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800">
+            <a:rPr lang="en-US" sz="1600" b="1">
               <a:solidFill>
-                <a:srgbClr val="7CEC66"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mj-lt"/>
             </a:rPr>
-            <a:t>Inventory List</a:t>
+            <a:t>2024</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr marL="0" algn="l"/>
           <a:r>
-            <a:rPr lang="en-US" sz="1800">
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
               <a:solidFill>
-                <a:srgbClr val="339933"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mj-lt"/>
             </a:rPr>
-            <a:t>DCS</a:t>
+            <a:t> Inventory Supplies</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="339933"/>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-            </a:rPr>
-            <a:t> OFFICE</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1800">
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
             <a:solidFill>
-              <a:srgbClr val="339933"/>
+              <a:schemeClr val="tx1"/>
             </a:solidFill>
             <a:latin typeface="+mj-lt"/>
           </a:endParaRPr>
@@ -645,16 +948,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>945527</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>282919</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>261666</xdr:rowOff>
+      <xdr:rowOff>182153</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>840874</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1018</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1303347</xdr:rowOff>
+      <xdr:rowOff>1223834</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -681,8 +984,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="2103767" y="261666"/>
-          <a:ext cx="1126142" cy="1041681"/>
+          <a:off x="2674936" y="182153"/>
+          <a:ext cx="1127799" cy="1041681"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -695,9 +998,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>762897</xdr:colOff>
+      <xdr:colOff>1220098</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>192502</xdr:rowOff>
+      <xdr:rowOff>139494</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3200400" cy="1211742"/>
     <xdr:sp macro="" textlink="">
@@ -713,7 +1016,494 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3330837" y="192502"/>
+          <a:off x="3612115" y="139494"/>
+          <a:ext cx="3200400" cy="1211742"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Republic of the Philippines</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CAVITE STATE UNIVERSITY</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>CCAT Campus</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Rosario, Cavite</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Wingdings 2" panose="05020102010507070707" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t></a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> (046) 437-9505 / </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:sym typeface="Wingdings 2" panose="05020102010507070707" pitchFamily="18" charset="2"/>
+            </a:rPr>
+            <a:t></a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" i="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>(046) 437-6659</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>cvsurosario@cvsu.edu.ph</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-PH" sz="1100" u="sng">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+              <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id=""/>
+            </a:rPr>
+            <a:t>www.cvsu-rosario.edu.ph</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>480059</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1440180</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>731520</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1737360</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1" descr="Inventory List" title="Title 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5135879" y="1440180"/>
+          <a:ext cx="2827021" cy="297180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="6350" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t>2024</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1600" b="1" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+            </a:rPr>
+            <a:t> Inventory Computer Lab </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1600" b="1">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:latin typeface="+mj-lt"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>282919</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>243113</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>122938</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1475294</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3650959" y="243113"/>
+          <a:ext cx="1127799" cy="1232181"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>244738</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101394</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3200400" cy="1211742"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4900558" y="101394"/>
           <a:ext cx="3200400" cy="1211742"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1044,23 +1834,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Inventory_List_Table" displayName="Inventory_List_Table" ref="B3:K13" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="B3:K13"/>
-  <tableColumns count="10">
-    <tableColumn id="1" name="For Reorder" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Inventory_List_Table" displayName="Inventory_List_Table" ref="B3:L13" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+  <autoFilter ref="B3:L13"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="For Reorder" dataDxfId="27">
       <calculatedColumnFormula>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Name" dataDxfId="10"/>
-    <tableColumn id="4" name="Description" dataDxfId="2"/>
-    <tableColumn id="5" name="Unit Price" dataDxfId="9" dataCellStyle="Currency"/>
-    <tableColumn id="6" name="Quantity in Stock" dataDxfId="8"/>
-    <tableColumn id="7" name="Inventory Value" dataDxfId="7">
+    <tableColumn id="2" name="Care of" dataDxfId="0"/>
+    <tableColumn id="3" name="Name" dataDxfId="26"/>
+    <tableColumn id="4" name="Description" dataDxfId="25"/>
+    <tableColumn id="5" name="Unit Price" dataDxfId="24" dataCellStyle="Currency"/>
+    <tableColumn id="6" name="Quantity in Stock" dataDxfId="23"/>
+    <tableColumn id="7" name="Inventory Value" dataDxfId="22">
       <calculatedColumnFormula>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" name="Reorder Level" dataDxfId="6"/>
-    <tableColumn id="9" name="Reorder Time in Days" dataDxfId="5"/>
-    <tableColumn id="10" name="Quantity in Reorder" dataDxfId="4"/>
-    <tableColumn id="11" name="Discontinued?" dataDxfId="3"/>
+    <tableColumn id="8" name="Reorder Level" dataDxfId="21"/>
+    <tableColumn id="9" name="Reorder Time in Days" dataDxfId="20"/>
+    <tableColumn id="10" name="Quantity in Reorder" dataDxfId="19"/>
+    <tableColumn id="11" name="Discontinued?" dataDxfId="18"/>
+  </tableColumns>
+  <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Inventory_List_Table3" displayName="Inventory_List_Table3" ref="A3:K8" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A3:K8"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="CCL" dataDxfId="15">
+      <calculatedColumnFormula>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="18" name="PC NO." dataDxfId="6"/>
+    <tableColumn id="3" name="Category" dataDxfId="7"/>
+    <tableColumn id="4" name="Brand" dataDxfId="5"/>
+    <tableColumn id="12" name="Model" dataDxfId="13"/>
+    <tableColumn id="13" name="Serial Number" dataDxfId="12"/>
+    <tableColumn id="14" name="Purchase Date" dataDxfId="11"/>
+    <tableColumn id="5" name="Unit Price" dataDxfId="14" dataCellStyle="Currency"/>
+    <tableColumn id="15" name="Warranty Expiry Date" dataDxfId="10" dataCellStyle="Currency"/>
+    <tableColumn id="16" name="Location " dataDxfId="9" dataCellStyle="Currency"/>
+    <tableColumn id="17" name="Condition" dataDxfId="8" dataCellStyle="Currency"/>
   </tableColumns>
   <tableStyleInfo name="Business Table" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1269,443 +2082,457 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:L17"/>
+  <dimension ref="B1:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.81640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12" style="2" customWidth="1"/>
-    <col min="3" max="3" width="14.7265625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="10.81640625" style="12" customWidth="1"/>
-    <col min="6" max="6" width="10.81640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="10" customWidth="1"/>
-    <col min="8" max="8" width="8.6328125" style="5" customWidth="1"/>
-    <col min="9" max="10" width="10.81640625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="1.81640625" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="8.81640625" style="3"/>
+    <col min="3" max="3" width="12" style="23" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.81640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.81640625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" style="5" customWidth="1"/>
+    <col min="10" max="11" width="10.81640625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="13" style="4" customWidth="1"/>
+    <col min="13" max="13" width="1.81640625" style="3" customWidth="1"/>
+    <col min="14" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" s="1" customFormat="1" ht="115.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
+    <row r="1" spans="2:13" s="1" customFormat="1" ht="141" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="6"/>
+    <row r="2" spans="2:13" ht="23.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D2" s="6"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="7"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="13"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:12" s="2" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" s="2" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="H3" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="I3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="L3" s="14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="12">
+      <c r="C4" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="12">
         <v>51</v>
       </c>
-      <c r="F4" s="5">
+      <c r="G4" s="5">
         <v>26</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>1326</v>
       </c>
-      <c r="H4" s="5">
+      <c r="I4" s="5">
         <v>69</v>
       </c>
-      <c r="I4" s="5">
+      <c r="J4" s="5">
         <v>13</v>
       </c>
-      <c r="J4" s="5">
+      <c r="K4" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="12">
+      <c r="C5" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="12">
         <v>93</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>132</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>12276</v>
       </c>
-      <c r="H5" s="5">
+      <c r="I5" s="5">
         <v>231</v>
       </c>
-      <c r="I5" s="5">
+      <c r="J5" s="5">
         <v>4</v>
       </c>
-      <c r="J5" s="5">
+      <c r="K5" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="D6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12">
         <v>57</v>
       </c>
-      <c r="F6" s="5">
+      <c r="G6" s="5">
         <v>151</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>8607</v>
       </c>
-      <c r="H6" s="5">
+      <c r="I6" s="5">
         <v>114</v>
       </c>
-      <c r="I6" s="5">
+      <c r="J6" s="5">
         <v>11</v>
       </c>
-      <c r="J6" s="5">
+      <c r="K6" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="17">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C7" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="19">
+      <c r="C7" s="17"/>
+      <c r="D7" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19">
         <v>19</v>
       </c>
-      <c r="F7" s="20">
+      <c r="G7" s="20">
         <v>191</v>
       </c>
-      <c r="G7" s="21">
+      <c r="H7" s="21">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>3629</v>
       </c>
-      <c r="H7" s="20">
+      <c r="I7" s="20">
         <v>190</v>
       </c>
-      <c r="I7" s="20">
+      <c r="J7" s="20">
         <v>6</v>
       </c>
-      <c r="J7" s="20">
+      <c r="K7" s="20">
         <v>50</v>
       </c>
-      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
     </row>
-    <row r="8" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="12">
         <v>75</v>
       </c>
-      <c r="F8" s="5">
+      <c r="G8" s="5">
         <v>62</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>4650</v>
       </c>
-      <c r="H8" s="5">
+      <c r="I8" s="5">
         <v>39</v>
       </c>
-      <c r="I8" s="5">
+      <c r="J8" s="5">
         <v>12</v>
       </c>
-      <c r="J8" s="5">
+      <c r="K8" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="12">
+        <v>11</v>
+      </c>
+      <c r="G9" s="5">
         <v>14</v>
       </c>
-      <c r="E9" s="12">
-        <v>11</v>
-      </c>
-      <c r="F9" s="5">
-        <v>14</v>
-      </c>
-      <c r="G9" s="10">
+      <c r="H9" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>154</v>
       </c>
-      <c r="H9" s="5">
+      <c r="I9" s="5">
         <v>9</v>
       </c>
-      <c r="I9" s="5">
+      <c r="J9" s="5">
         <v>13</v>
       </c>
-      <c r="J9" s="5">
+      <c r="K9" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="10" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="12">
+      <c r="D10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="12">
         <v>56</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>58</v>
       </c>
-      <c r="G10" s="10">
+      <c r="H10" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>3248</v>
       </c>
-      <c r="H10" s="5">
+      <c r="I10" s="5">
         <v>109</v>
       </c>
-      <c r="I10" s="5">
+      <c r="J10" s="5">
         <v>7</v>
       </c>
-      <c r="J10" s="5">
+      <c r="K10" s="5">
         <v>100</v>
       </c>
-      <c r="K10" s="4" t="s">
+      <c r="L10" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="12">
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" s="12">
         <v>38</v>
       </c>
-      <c r="F11" s="5">
+      <c r="G11" s="5">
         <v>101</v>
       </c>
-      <c r="G11" s="10">
+      <c r="H11" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>3838</v>
       </c>
-      <c r="H11" s="5">
+      <c r="I11" s="5">
         <v>162</v>
       </c>
-      <c r="I11" s="5">
+      <c r="J11" s="5">
         <v>3</v>
       </c>
-      <c r="J11" s="5">
+      <c r="K11" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>0</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="12">
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="12">
         <v>59</v>
       </c>
-      <c r="F12" s="5">
+      <c r="G12" s="5">
         <v>122</v>
       </c>
-      <c r="G12" s="10">
+      <c r="H12" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>7198</v>
       </c>
-      <c r="H12" s="5">
+      <c r="I12" s="5">
         <v>82</v>
       </c>
-      <c r="I12" s="5">
+      <c r="J12" s="5">
         <v>3</v>
       </c>
-      <c r="J12" s="5">
+      <c r="K12" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <f>IFERROR((Inventory_List_Table[[#This Row],[Quantity in Stock]]&lt;=Inventory_List_Table[[#This Row],[Reorder Level]])*(Inventory_List_Table[[#This Row],[Discontinued?]]="")*valHighlight,0)</f>
         <v>1</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="12">
+      <c r="D13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="12">
         <v>50</v>
       </c>
-      <c r="F13" s="5">
+      <c r="G13" s="5">
         <v>175</v>
       </c>
-      <c r="G13" s="10">
+      <c r="H13" s="10">
         <f>Inventory_List_Table[[#This Row],[Unit Price]]*Inventory_List_Table[[#This Row],[Quantity in Stock]]</f>
         <v>8750</v>
       </c>
-      <c r="H13" s="5">
+      <c r="I13" s="5">
         <v>283</v>
       </c>
-      <c r="I13" s="5">
+      <c r="J13" s="5">
         <v>8</v>
       </c>
-      <c r="J13" s="5">
+      <c r="K13" s="5">
         <v>150</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:13" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K15" s="3"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="22"/>
+      <c r="K16" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="L16" s="25"/>
     </row>
-    <row r="16" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="24" t="s">
+    <row r="17" spans="2:12" ht="24" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="22"/>
-      <c r="J16" s="24" t="s">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="22"/>
+      <c r="K17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="K16" s="24"/>
-    </row>
-    <row r="17" spans="2:11" ht="24" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="22"/>
-      <c r="J17" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K17" s="24"/>
+      <c r="L17" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K17:L17"/>
   </mergeCells>
-  <conditionalFormatting sqref="B4:K13">
-    <cfRule type="expression" dxfId="1" priority="24">
-      <formula>$K4="Yes"</formula>
+  <conditionalFormatting sqref="B4:L13">
+    <cfRule type="expression" dxfId="4" priority="24">
+      <formula>$L4="Yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="25">
+    <cfRule type="expression" dxfId="3" priority="25">
       <formula>$B4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations xWindow="67" yWindow="628" count="13">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Inventory List" prompt="_x000a_This worksheet tracks inventory for items listed in the inventory list table and contains the ability to highlight and flag those items that are ready to be reordered. Discontinued items have strikethrough formatting and a Yes in the Discontinued column." sqref="A2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an automated column. _x000a__x000a_A flag icon in this column indicates items in the inventory list that are ready to be reordered. Flag icons only appear when a Yes is selected in L2 and the item meets the reorder criteria." sqref="B3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the item in this column" sqref="C3:D3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter yes if the item has been discontinued. When a yes is entered, the corresponding row is highlighted a light grey and the font style changed to strikethrough" sqref="K3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the quantity in reorder for each item in this column" sqref="J3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the number of days it takes to reorder each item in this column" sqref="I3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the reorder level for each item in this column" sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an automated column._x000a__x000a_The inventory value for each item is automatically calculated in this column." sqref="G3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the quantity in stock for each item in this column" sqref="F3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the unit price of each item in this column" sqref="E3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K4:K13">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an automated column. _x000a__x000a_A flag icon in this column indicates items in the inventory list that are ready to be reordered. Flag icons only appear when a Yes is selected in L2 and the item meets the reorder criteria." sqref="B3:C3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the item in this column" sqref="D3:E3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter yes if the item has been discontinued. When a yes is entered, the corresponding row is highlighted a light grey and the font style changed to strikethrough" sqref="L3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the quantity in reorder for each item in this column" sqref="K3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the number of days it takes to reorder each item in this column" sqref="J3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the reorder level for each item in this column" sqref="I3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an automated column._x000a__x000a_The inventory value for each item is automatically calculated in this column." sqref="H3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the quantity in stock for each item in this column" sqref="G3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the unit price of each item in this column" sqref="F3"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L4:L13">
       <formula1>"Yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes to enable highlighting of items for reorder. This will put a flag in column B and highlight the corresponding row in the Inventory List table.  Selecting No clears the flag and all highlights." sqref="K2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select Yes to enable highlighting of items for reorder. This will put a flag in column B and highlight the corresponding row in the Inventory List table.  Selecting No clears the flag and all highlights." sqref="L2">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Inventory List" prompt="This worksheet tracks inventory for items listed in the inventory list table and contains the ability to highlight and flag those items that are ready to be reordered. Discontinued items have strikethrough formatting and a Yes in the Discontinued column." sqref="A1"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="82" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="65" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <tableParts count="1">
     <tablePart r:id="rId3"/>
@@ -1730,11 +2557,264 @@
               <x14:cfIcon iconSet="3Flags" iconId="0"/>
             </x14:iconSet>
           </x14:cfRule>
-          <xm:sqref>B4:B13</xm:sqref>
+          <xm:sqref>B4:C13</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="10.54296875" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" customWidth="1"/>
+    <col min="4" max="7" width="15.36328125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="21.1796875" customWidth="1"/>
+    <col min="10" max="11" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="158.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="23">
+        <f>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B4" s="23"/>
+      <c r="C4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="12">
+        <v>51</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="23">
+        <f>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="12">
+        <v>93</v>
+      </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="23">
+        <f>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="12">
+        <v>57</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="17">
+        <f>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19">
+        <v>19</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="23">
+        <f>IFERROR((#REF!&lt;=#REF!)*(#REF!="")*valHighlight,0)</f>
+        <v>0</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="12">
+        <v>75</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="A4:K8">
+    <cfRule type="expression" dxfId="2" priority="33">
+      <formula>$L4="Yes"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="34">
+      <formula>$C4=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the unit price of each item in this column" sqref="H3:K3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the name of the item in this column" sqref="C3:G3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This is an automated column. _x000a__x000a_A flag icon in this column indicates items in the inventory list that are ready to be reordered. Flag icons only appear when a Yes is selected in L2 and the item meets the reorder criteria." sqref="A3:B3"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="35" id="{32031D6E-9839-4734-B466-5B2246B77D37}">
+            <x14:iconSet showValue="0" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>-1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="NoIcons" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>A4:B8</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1748,15 +2828,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DEEA25CC0A0AC24199CDC46C25B8B0BC" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e3b47856d4cf355c0dacb39e1084d14f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="6dc4bcd6-49db-4c07-9060-8acfc67cef9f" xmlns:ns3="fb0879af-3eba-417a-a55a-ffe6dcd6ca77" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a845a615265fdb1f7b12cc65ac20ecbd" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1964,6 +3035,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE17AD16-C3BD-472A-B362-8A85F95573CA}">
   <ds:schemaRefs>
@@ -1973,24 +3053,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1227E31-123E-44EE-A422-2705DF3A5917}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2008,4 +3070,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{81F3298A-223B-42B2-9FEF-AB506EA6B5F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6dc4bcd6-49db-4c07-9060-8acfc67cef9f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="fb0879af-3eba-417a-a55a-ffe6dcd6ca77"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>